<commit_message>
update test trending dashboard to diagnose balance
</commit_message>
<xml_diff>
--- a/Documentation/robot-network-table-list.xlsx
+++ b/Documentation/robot-network-table-list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
   <si>
     <t xml:space="preserve">system</t>
   </si>
@@ -147,20 +147,49 @@
   </si>
   <si>
     <t xml:space="preserve">should this be part of human… (the modifier probably should only apply to joystick driving…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/Err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/RateOfChange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/ErrAdj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/SpeedDmdRaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/SpeedDmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/RateOfChangeRaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to add </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance/ExeCount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -239,33 +268,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -277,29 +310,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -370,8 +380,8 @@
   </sheetPr>
   <dimension ref="C4:F56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,44 +758,74 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E43" s="5"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E44" s="5"/>
-      <c r="F44" s="6"/>
+      <c r="F44" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="6"/>
     </row>
@@ -880,26 +920,26 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="7" t="n">
         <f aca="false">6+1/2</f>
         <v>6.5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="7" t="n">
         <f aca="false">C3*PI()/12</f>
         <v>1.70169602069447</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="7" t="n">
         <f aca="false">D3/C4/C5</f>
         <v>0.00118173334770449</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="7" t="n">
         <v>360</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="7" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>